<commit_message>
Màj excels avec les données Rugby et Baseball
</commit_message>
<xml_diff>
--- a/Donnees_Bless_Poles.xlsx
+++ b/Donnees_Bless_Poles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e3e93a7e0c88a78/Documents/INSA_4_GMM/Semestre 2/Projet tutoré/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e3e93a7e0c88a78/Documents/INSA_4_GMM/Semestre 2/Projet tutoré/Projet_CREPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{1F727089-CAAB-4369-99FF-DC8542B01161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2D71760F-A57F-412A-B701-86FDBD222E4B}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{1F727089-CAAB-4369-99FF-DC8542B01161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1E8CBE74-EE2A-41FA-984B-A04D01DCE990}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="2505" windowWidth="15375" windowHeight="7875" xr2:uid="{C863FA4C-14E0-41CD-8273-920CE2A6FD88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C863FA4C-14E0-41CD-8273-920CE2A6FD88}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>POLE</t>
   </si>
   <si>
-    <t>NB_BLESSURES</t>
-  </si>
-  <si>
     <t>AV</t>
   </si>
   <si>
@@ -64,6 +61,15 @@
   </si>
   <si>
     <t>BLESS_POURC</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>NB_BLESSES</t>
+  </si>
+  <si>
+    <t>BS</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187D59DF-2E04-4A91-A99A-AE0DC0119A8D}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,18 +441,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>13</v>
@@ -461,7 +467,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -470,13 +476,13 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D7" si="0">(B3/C3)*100</f>
+        <f t="shared" ref="D3:D9" si="0">(B3/C3)*100</f>
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -491,7 +497,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -506,7 +512,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>13</v>
@@ -521,17 +527,47 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
         <v>4</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.666666666666668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>80.952380952380949</v>
       </c>
     </row>
   </sheetData>

</xml_diff>